<commit_message>
fix: nameless vuz in templan and ntp xlsx tables
</commit_message>
<xml_diff>
--- a/DB/Ntp_pr.xlsx
+++ b/DB/Ntp_pr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\PyProj\subd\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programs\PyProjects\subd\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C183F22-2717-466F-BD92-838212FCD1B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CCD98C-89D7-4701-8B4C-1EFABF12FFC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="1327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="1328">
   <si>
     <t>UniqueID</t>
   </si>
@@ -4006,6 +4006,9 @@
   </si>
   <si>
     <t>Р</t>
+  </si>
+  <si>
+    <t>ГУУ</t>
   </si>
 </sst>
 </file>
@@ -4333,8 +4336,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.8984375" customWidth="1"/>
+    <col min="11" max="11" width="27.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -5188,7 +5191,10 @@
         <v>35</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
       </c>
       <c r="F25" t="s">
         <v>96</v>
@@ -5255,7 +5261,10 @@
         <v>48</v>
       </c>
       <c r="D27">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
       </c>
       <c r="F27" t="s">
         <v>98</v>
@@ -5917,7 +5926,10 @@
         <v>1</v>
       </c>
       <c r="D46">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
       </c>
       <c r="F46" t="s">
         <v>113</v>
@@ -6614,7 +6626,10 @@
         <v>16</v>
       </c>
       <c r="D66">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E66" t="s">
+        <v>7</v>
       </c>
       <c r="F66" t="s">
         <v>130</v>
@@ -7276,7 +7291,10 @@
         <v>6</v>
       </c>
       <c r="D85">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="E85" t="s">
+        <v>66</v>
       </c>
       <c r="F85" t="s">
         <v>147</v>
@@ -9758,7 +9776,10 @@
         <v>2</v>
       </c>
       <c r="D156">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E156" t="s">
+        <v>7</v>
       </c>
       <c r="F156" t="s">
         <v>198</v>
@@ -11680,7 +11701,10 @@
         <v>4</v>
       </c>
       <c r="D211">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="E211" t="s">
+        <v>66</v>
       </c>
       <c r="F211" t="s">
         <v>100</v>
@@ -12482,7 +12506,10 @@
         <v>2</v>
       </c>
       <c r="D234">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E234" t="s">
+        <v>7</v>
       </c>
       <c r="F234" t="s">
         <v>129</v>
@@ -12549,7 +12576,10 @@
         <v>9</v>
       </c>
       <c r="D236">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="E236" t="s">
+        <v>1327</v>
       </c>
       <c r="F236" t="s">
         <v>103</v>
@@ -15626,7 +15656,10 @@
         <v>26</v>
       </c>
       <c r="D324">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="E324" t="s">
+        <v>66</v>
       </c>
       <c r="F324" t="s">
         <v>298</v>
@@ -15728,7 +15761,10 @@
         <v>3</v>
       </c>
       <c r="D327">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="E327" t="s">
+        <v>19</v>
       </c>
       <c r="F327" t="s">
         <v>101</v>
@@ -17440,7 +17476,10 @@
         <v>28</v>
       </c>
       <c r="D376">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="E376" t="s">
+        <v>66</v>
       </c>
       <c r="F376" t="s">
         <v>122</v>
@@ -18337,6 +18376,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K401">
+    <sortCondition ref="A2:A401"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>